<commit_message>
Bfr new benchmark tests.
</commit_message>
<xml_diff>
--- a/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
+++ b/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madks\Documents\GitHub\Ozone-Narx-DNN\models\NarxModelSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E59600E-AB2B-4864-80B7-6FEEDDF60190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA97ECD1-47D4-4562-9FA5-1FE1E80B8B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18720" activeTab="3" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
   </bookViews>
@@ -5995,7 +5995,7 @@
   <dimension ref="E1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Several math benchmarks 20 islands done. Bfr "noX" benchmarks. Bfr MT 3 countries
</commit_message>
<xml_diff>
--- a/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
+++ b/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madks\Documents\GitHub\Ozone-Narx-DNN\models\NarxModelSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41F49D-17D5-4D03-BB72-BB5F8E2FDD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B28A403-CEAD-49BB-A5DD-F465679ADDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="6" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="783" activeTab="6" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosenbrock" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="T-testResults" sheetId="8" r:id="rId5"/>
     <sheet name="MT_CY_DMtests" sheetId="10" r:id="rId6"/>
     <sheet name="AblationAverages" sheetId="13" r:id="rId7"/>
+    <sheet name="AblationAveragesReduced" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3802" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3869" uniqueCount="142">
   <si>
     <t>ackley</t>
   </si>
@@ -451,12 +452,48 @@
   <si>
     <t>on "3x {BO} 2x {PSO} 1x {Rand, GA, DE}"</t>
   </si>
+  <si>
+    <t>Accuracy (rank out of 6):</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>PSO</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>total islands</t>
+  </si>
+  <si>
+    <t>Expected ratios:</t>
+  </si>
+  <si>
+    <t>Island counts:</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>on "4x {BO} ,1x {PSO, Rand, GA, DE}"</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,6 +520,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -695,10 +739,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -733,10 +778,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -745,13 +791,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1065,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CE41FD-81F2-4685-81AA-A855FD795D3A}">
   <dimension ref="A1:AA278"/>
   <sheetViews>
-    <sheetView topLeftCell="E229" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AB271" sqref="AB271"/>
     </sheetView>
   </sheetViews>
@@ -61339,10 +61391,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CEA5EE-3BD5-4281-8B13-E05FA0E89401}">
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -61419,7 +61471,7 @@
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="47" t="s">
         <v>119</v>
       </c>
       <c r="F3" s="33"/>
@@ -61447,7 +61499,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="40"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="8" t="s">
         <v>43</v>
       </c>
@@ -61490,35 +61542,35 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="33"/>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="39" t="s">
         <v>97</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="39" t="s">
         <v>98</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="40" t="s">
         <v>97</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="39" t="s">
         <v>98</v>
       </c>
       <c r="M5" s="11"/>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="39" t="s">
         <v>97</v>
       </c>
       <c r="O5" s="9"/>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="39" t="s">
         <v>98</v>
       </c>
       <c r="Q5" s="11"/>
-      <c r="R5" s="39" t="s">
+      <c r="R5" s="40" t="s">
         <v>97</v>
       </c>
       <c r="S5" s="9"/>
-      <c r="T5" s="38" t="s">
+      <c r="T5" s="39" t="s">
         <v>98</v>
       </c>
       <c r="U5" s="11"/>
@@ -61634,7 +61686,7 @@
         <f>Rastrigin!P106</f>
         <v>34.28</v>
       </c>
-      <c r="P7" s="43">
+      <c r="P7" s="44">
         <f>Rastrigin!N107</f>
         <v>8.98</v>
       </c>
@@ -61678,7 +61730,7 @@
         <f>Rosenbrock!Y106</f>
         <v>13708.52</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="43">
         <f>Rosenbrock!W107</f>
         <v>9.02</v>
       </c>
@@ -61802,7 +61854,7 @@
         <f>Schaffer!G141</f>
         <v>54.34</v>
       </c>
-      <c r="T9" s="42">
+      <c r="T9" s="43">
         <f>Schaffer!E142</f>
         <v>8.02</v>
       </c>
@@ -61895,7 +61947,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="37" t="s">
         <v>111</v>
       </c>
       <c r="F11" s="12">
@@ -61922,7 +61974,7 @@
         <f>Ackley!Y141</f>
         <v>0.51</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="43">
         <f>Ackley!W142</f>
         <v>8.86</v>
       </c>
@@ -61982,7 +62034,7 @@
         <f>Rosenbrock!G176</f>
         <v>2851.84</v>
       </c>
-      <c r="H12" s="43">
+      <c r="H12" s="44">
         <f>Rosenbrock!E177</f>
         <v>8.69</v>
       </c>
@@ -62275,7 +62327,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="37" t="s">
         <v>118</v>
       </c>
       <c r="F16" s="12">
@@ -62302,7 +62354,7 @@
         <f>Ackley!P211</f>
         <v>0.25</v>
       </c>
-      <c r="L16" s="42">
+      <c r="L16" s="43">
         <f>Ackley!N212</f>
         <v>8.57</v>
       </c>
@@ -62427,7 +62479,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="37" t="s">
         <v>124</v>
       </c>
       <c r="F18" s="12">
@@ -62503,7 +62555,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="38" t="s">
         <v>128</v>
       </c>
       <c r="F19" s="14">
@@ -62530,7 +62582,7 @@
         <f>Ackley!P246</f>
         <v>0.68</v>
       </c>
-      <c r="L19" s="47">
+      <c r="L19" s="48">
         <f>Ackley!N247</f>
         <v>8.3699999999999992</v>
       </c>
@@ -62538,7 +62590,7 @@
         <f>Ackley!P247</f>
         <v>0.45</v>
       </c>
-      <c r="N19" s="41">
+      <c r="N19" s="42">
         <f>Rastrigin!N246</f>
         <v>618.09</v>
       </c>
@@ -62605,7 +62657,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="45" t="s">
         <v>106</v>
       </c>
       <c r="F21" t="s">
@@ -62620,7 +62672,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="46" t="s">
         <v>122</v>
       </c>
       <c r="F22" s="29">
@@ -62656,7 +62708,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="46" t="s">
         <v>121</v>
       </c>
       <c r="F23" s="29"/>
@@ -62692,7 +62744,7 @@
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="46" t="s">
         <v>105</v>
       </c>
       <c r="F24" s="29"/>
@@ -62766,7 +62818,7 @@
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="45" t="s">
         <v>106</v>
       </c>
       <c r="F26" t="s">
@@ -62777,7 +62829,7 @@
       <c r="X26" s="7"/>
     </row>
     <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E27" s="45" t="s">
+      <c r="E27" s="46" t="s">
         <v>122</v>
       </c>
       <c r="F27" s="29">
@@ -62806,7 +62858,7 @@
       <c r="U27" s="31"/>
     </row>
     <row r="28" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="46" t="s">
         <v>126</v>
       </c>
       <c r="F28" s="29"/>
@@ -62847,7 +62899,7 @@
       </c>
     </row>
     <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="45" t="s">
         <v>106</v>
       </c>
       <c r="F30" t="s">
@@ -62855,7 +62907,7 @@
       </c>
     </row>
     <row r="31" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="46" t="s">
         <v>122</v>
       </c>
       <c r="F31" s="29">
@@ -62884,7 +62936,7 @@
       <c r="U31" s="31"/>
     </row>
     <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E32" s="45" t="s">
+      <c r="E32" s="46" t="s">
         <v>126</v>
       </c>
       <c r="F32" s="29"/>
@@ -62924,8 +62976,1016 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E37" s="1"/>
+    <row r="36" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E37" s="27">
+        <v>8</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G37" t="s">
+        <v>140</v>
+      </c>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="31"/>
+    </row>
+    <row r="38" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E38" s="17"/>
+      <c r="F38" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="K38" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E39" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="17">
+        <v>4</v>
+      </c>
+      <c r="G39" s="9">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9">
+        <v>1</v>
+      </c>
+      <c r="I39" s="9">
+        <v>1</v>
+      </c>
+      <c r="J39" s="11">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <f>SUM(F39:J39)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E40" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="53">
+        <f>F39/$E$37</f>
+        <v>0.5</v>
+      </c>
+      <c r="G40" s="51">
+        <f>G39/$E$37</f>
+        <v>0.125</v>
+      </c>
+      <c r="H40" s="51">
+        <f>H39/$E$37</f>
+        <v>0.125</v>
+      </c>
+      <c r="I40" s="51">
+        <f>I39/$E$37</f>
+        <v>0.125</v>
+      </c>
+      <c r="J40" s="52">
+        <f>J39/$E$37</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F42">
+        <v>0.1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="27">
+        <v>8</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G44" t="s">
+        <v>129</v>
+      </c>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="31"/>
+    </row>
+    <row r="45" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E45" s="17"/>
+      <c r="F45" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I45" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="J45" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="K45" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E46" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" s="17">
+        <v>2</v>
+      </c>
+      <c r="G46" s="9">
+        <v>2</v>
+      </c>
+      <c r="H46" s="9">
+        <v>2</v>
+      </c>
+      <c r="I46" s="9">
+        <v>1</v>
+      </c>
+      <c r="J46" s="11">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <f>SUM(F46:J46)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E47" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="53">
+        <f>F46/$E$37</f>
+        <v>0.25</v>
+      </c>
+      <c r="G47" s="51">
+        <f>G46/$E$37</f>
+        <v>0.25</v>
+      </c>
+      <c r="H47" s="51">
+        <f>H46/$E$37</f>
+        <v>0.25</v>
+      </c>
+      <c r="I47" s="51">
+        <f>I46/$E$37</f>
+        <v>0.125</v>
+      </c>
+      <c r="J47" s="52">
+        <f>J46/$E$37</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49">
+        <v>0.1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9560DDCE-6A26-4DFC-8300-4EAE2EB40D3A}">
+  <dimension ref="A1:X17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="29.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.90625" customWidth="1"/>
+    <col min="18" max="18" width="14.6328125" customWidth="1"/>
+    <col min="19" max="19" width="12.08984375" customWidth="1"/>
+    <col min="20" max="20" width="11.90625" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+    </row>
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+    </row>
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="S4" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="S5" s="9"/>
+      <c r="T5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="U5" s="11"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+    </row>
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="17">
+        <f>Rosenbrock!N106</f>
+        <v>40455.75</v>
+      </c>
+      <c r="G7" s="9">
+        <f>Rosenbrock!P106</f>
+        <v>6752.81</v>
+      </c>
+      <c r="H7" s="17">
+        <f>Rosenbrock!N107</f>
+        <v>9.15</v>
+      </c>
+      <c r="I7" s="11">
+        <f>Rosenbrock!P107</f>
+        <v>0.3</v>
+      </c>
+      <c r="J7" s="9">
+        <f>Ackley!N106</f>
+        <v>19.29</v>
+      </c>
+      <c r="K7" s="9">
+        <f>Ackley!P106</f>
+        <v>0.37</v>
+      </c>
+      <c r="L7" s="17">
+        <f>Ackley!N107</f>
+        <v>8.92</v>
+      </c>
+      <c r="M7" s="11">
+        <f>Ackley!P107</f>
+        <v>0.38</v>
+      </c>
+      <c r="N7" s="17">
+        <f>Rastrigin!N106</f>
+        <v>693.85</v>
+      </c>
+      <c r="O7" s="9">
+        <f>Rastrigin!P106</f>
+        <v>34.28</v>
+      </c>
+      <c r="P7" s="44">
+        <f>Rastrigin!N107</f>
+        <v>8.98</v>
+      </c>
+      <c r="Q7" s="11">
+        <f>Rastrigin!P107</f>
+        <v>0.23</v>
+      </c>
+      <c r="R7" s="9">
+        <f>Schaffer!N106</f>
+        <v>505.01</v>
+      </c>
+      <c r="S7" s="9">
+        <f>Schaffer!P106</f>
+        <v>19.27</v>
+      </c>
+      <c r="T7" s="17">
+        <f>Schaffer!N107</f>
+        <v>8.07</v>
+      </c>
+      <c r="U7" s="11">
+        <f>Schaffer!P107</f>
+        <v>0.23</v>
+      </c>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="43">
+        <f>Rosenbrock!W106</f>
+        <v>25543.46</v>
+      </c>
+      <c r="G8" s="7">
+        <f>Rosenbrock!Y106</f>
+        <v>13708.52</v>
+      </c>
+      <c r="H8" s="43">
+        <f>Rosenbrock!W107</f>
+        <v>9.02</v>
+      </c>
+      <c r="I8" s="13">
+        <f>Rosenbrock!Y107</f>
+        <v>0.51</v>
+      </c>
+      <c r="J8" s="7">
+        <f>Ackley!W106</f>
+        <v>19.27</v>
+      </c>
+      <c r="K8" s="7">
+        <f>Ackley!Y106</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L8" s="12">
+        <f>Ackley!W107</f>
+        <v>8.98</v>
+      </c>
+      <c r="M8" s="13">
+        <f>Ackley!Y107</f>
+        <v>0.36</v>
+      </c>
+      <c r="N8" s="12">
+        <f>Rastrigin!W106</f>
+        <v>635.84</v>
+      </c>
+      <c r="O8" s="7">
+        <f>Rastrigin!Y106</f>
+        <v>87.64</v>
+      </c>
+      <c r="P8" s="12">
+        <f>Rastrigin!W107</f>
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="Q8" s="13">
+        <f>Rastrigin!Y107</f>
+        <v>0.32</v>
+      </c>
+      <c r="R8" s="25">
+        <f>Schaffer!W106</f>
+        <v>471.38</v>
+      </c>
+      <c r="S8" s="7">
+        <f>Schaffer!Y106</f>
+        <v>59.64</v>
+      </c>
+      <c r="T8" s="12">
+        <f>Schaffer!W107</f>
+        <v>8.07</v>
+      </c>
+      <c r="U8" s="13">
+        <f>Schaffer!Y107</f>
+        <v>0.21</v>
+      </c>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="12">
+        <f>Rosenbrock!E141</f>
+        <v>28047.98</v>
+      </c>
+      <c r="G9" s="7">
+        <f>Rosenbrock!G141</f>
+        <v>14114.72</v>
+      </c>
+      <c r="H9" s="12">
+        <f>Rosenbrock!E142</f>
+        <v>9.09</v>
+      </c>
+      <c r="I9" s="13">
+        <f>Rosenbrock!G142</f>
+        <v>0.4</v>
+      </c>
+      <c r="J9" s="7">
+        <f>Ackley!E141</f>
+        <v>19.190000000000001</v>
+      </c>
+      <c r="K9" s="13">
+        <f>Ackley!G141</f>
+        <v>0.48</v>
+      </c>
+      <c r="L9" s="12">
+        <f>Ackley!E142</f>
+        <v>9.08</v>
+      </c>
+      <c r="M9" s="13">
+        <f>Ackley!G142</f>
+        <v>0.41</v>
+      </c>
+      <c r="N9" s="12">
+        <f>Rastrigin!E141</f>
+        <v>649.87</v>
+      </c>
+      <c r="O9" s="7">
+        <f>Rastrigin!G141</f>
+        <v>71.47</v>
+      </c>
+      <c r="P9" s="12">
+        <f>Rastrigin!E142</f>
+        <v>9.1</v>
+      </c>
+      <c r="Q9" s="13">
+        <f>Rastrigin!G142</f>
+        <v>0.23</v>
+      </c>
+      <c r="R9" s="24">
+        <f>Schaffer!E141</f>
+        <v>465.22</v>
+      </c>
+      <c r="S9" s="7">
+        <f>Schaffer!G141</f>
+        <v>54.34</v>
+      </c>
+      <c r="T9" s="43">
+        <f>Schaffer!E142</f>
+        <v>8.02</v>
+      </c>
+      <c r="U9" s="13">
+        <f>Schaffer!G142</f>
+        <v>0.32</v>
+      </c>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="12">
+        <f>Rosenbrock!N141</f>
+        <v>25861.86</v>
+      </c>
+      <c r="G10" s="7">
+        <f>Rosenbrock!P141</f>
+        <v>12143.24</v>
+      </c>
+      <c r="H10" s="12">
+        <f>Rosenbrock!N142</f>
+        <v>9.08</v>
+      </c>
+      <c r="I10" s="13">
+        <f>Rosenbrock!P142</f>
+        <v>0.4</v>
+      </c>
+      <c r="J10" s="24">
+        <f>Ackley!N141</f>
+        <v>18.940000000000001</v>
+      </c>
+      <c r="K10" s="13">
+        <f>Ackley!P141</f>
+        <v>0.66</v>
+      </c>
+      <c r="L10" s="12">
+        <f>Ackley!N142</f>
+        <v>9.07</v>
+      </c>
+      <c r="M10" s="13">
+        <f>Ackley!P142</f>
+        <v>0.37</v>
+      </c>
+      <c r="N10" s="12">
+        <f>Rastrigin!N141</f>
+        <v>626.57000000000005</v>
+      </c>
+      <c r="O10" s="7">
+        <f>Rastrigin!P141</f>
+        <v>86.68</v>
+      </c>
+      <c r="P10" s="12">
+        <f>Rastrigin!N142</f>
+        <v>9.08</v>
+      </c>
+      <c r="Q10" s="13">
+        <f>Rastrigin!P142</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R10" s="7">
+        <f>Schaffer!N141</f>
+        <v>471.51</v>
+      </c>
+      <c r="S10" s="7">
+        <f>Schaffer!P141</f>
+        <v>52.05</v>
+      </c>
+      <c r="T10" s="12">
+        <f>Schaffer!N142</f>
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="U10" s="13">
+        <f>Schaffer!P142</f>
+        <v>0.31</v>
+      </c>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+    </row>
+    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="12">
+        <f>Rosenbrock!W141</f>
+        <v>31222.59</v>
+      </c>
+      <c r="G11" s="7">
+        <f>Rosenbrock!Y141</f>
+        <v>12983.88</v>
+      </c>
+      <c r="H11" s="12">
+        <f>Rosenbrock!W142</f>
+        <v>9.11</v>
+      </c>
+      <c r="I11" s="13">
+        <f>Rosenbrock!Y142</f>
+        <v>0.44</v>
+      </c>
+      <c r="J11" s="7">
+        <f>Ackley!W141</f>
+        <v>19.170000000000002</v>
+      </c>
+      <c r="K11" s="13">
+        <f>Ackley!Y141</f>
+        <v>0.51</v>
+      </c>
+      <c r="L11" s="43">
+        <f>Ackley!W142</f>
+        <v>8.86</v>
+      </c>
+      <c r="M11" s="13">
+        <f>Ackley!Y142</f>
+        <v>0.21</v>
+      </c>
+      <c r="N11" s="33">
+        <f>Rastrigin!W141</f>
+        <v>621.27</v>
+      </c>
+      <c r="O11" s="7">
+        <f>Rastrigin!Y141</f>
+        <v>88.8</v>
+      </c>
+      <c r="P11" s="12">
+        <f>Rastrigin!W142</f>
+        <v>9.02</v>
+      </c>
+      <c r="Q11" s="13">
+        <f>Rastrigin!Y142</f>
+        <v>0.23</v>
+      </c>
+      <c r="R11" s="7">
+        <f>Schaffer!W141</f>
+        <v>492.13</v>
+      </c>
+      <c r="S11" s="7">
+        <f>Schaffer!Y141</f>
+        <v>50.07</v>
+      </c>
+      <c r="T11" s="12">
+        <f>Schaffer!W142</f>
+        <v>8.11</v>
+      </c>
+      <c r="U11" s="13">
+        <f>Schaffer!Y142</f>
+        <v>0.38</v>
+      </c>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+    </row>
+    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="49">
+        <f>Rosenbrock!E1</f>
+        <v>17604.830000000002</v>
+      </c>
+      <c r="G12" s="31">
+        <f>Rosenbrock!G1</f>
+        <v>10654.88</v>
+      </c>
+      <c r="H12" s="50">
+        <f>Rosenbrock!E34</f>
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="I12" s="29">
+        <f>Rosenbrock!G34</f>
+        <v>1.56</v>
+      </c>
+      <c r="J12" s="27">
+        <f>Ackley!E1</f>
+        <v>19</v>
+      </c>
+      <c r="K12" s="31">
+        <f>Ackley!G1</f>
+        <v>0.43</v>
+      </c>
+      <c r="L12" s="50">
+        <f>Ackley!E34</f>
+        <v>7.8</v>
+      </c>
+      <c r="M12" s="29">
+        <f>Ackley!G34</f>
+        <v>0.05</v>
+      </c>
+      <c r="N12" s="27">
+        <f>Rastrigin!E1</f>
+        <v>625.92999999999995</v>
+      </c>
+      <c r="O12" s="31">
+        <f>Rastrigin!G1</f>
+        <v>72.760000000000005</v>
+      </c>
+      <c r="P12" s="50">
+        <f>Rastrigin!E34</f>
+        <v>7.97</v>
+      </c>
+      <c r="Q12" s="29">
+        <f>Rastrigin!G34</f>
+        <v>0.38</v>
+      </c>
+      <c r="R12" s="27">
+        <f>Schaffer!E1</f>
+        <v>473.75</v>
+      </c>
+      <c r="S12" s="31">
+        <f>Schaffer!G1</f>
+        <v>46.38</v>
+      </c>
+      <c r="T12" s="50">
+        <f>Schaffer!E34</f>
+        <v>7.85</v>
+      </c>
+      <c r="U12" s="31">
+        <f>Schaffer!G34</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+    </row>
+    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="29">
+        <v>1</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="27">
+        <v>2</v>
+      </c>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="29">
+        <v>2</v>
+      </c>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="27">
+        <v>4</v>
+      </c>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="X17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Paper RC3. Submitted R2.
</commit_message>
<xml_diff>
--- a/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
+++ b/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madks\Documents\GitHub\Ozone-Narx-DNN\models\NarxModelSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04061CB9-FE3F-4C64-9165-E92E0AEA0A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C919F68-0D22-4363-B8DF-01EF1723F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15370" tabRatio="440" activeTab="4" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
+    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18720" tabRatio="440" activeTab="4" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosenbrock" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3946" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="145">
   <si>
     <t>ackley</t>
   </si>
@@ -490,6 +490,12 @@
   </si>
   <si>
     <t>Execution time (non-communicating)</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Lines that can be reduced</t>
   </si>
 </sst>
 </file>
@@ -59600,10 +59606,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB09A27-0144-4906-BC0E-BB2A5E88B564}">
-  <dimension ref="E1:N42"/>
+  <dimension ref="D1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -60349,7 +60355,7 @@
         <v>0.96819999999999995</v>
       </c>
     </row>
-    <row r="33" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.35">
       <c r="F33">
         <v>2.74</v>
       </c>
@@ -60369,7 +60375,7 @@
         <v>3.39</v>
       </c>
     </row>
-    <row r="34" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.35">
       <c r="F34">
         <v>6.5305223769944899E-3</v>
       </c>
@@ -60389,7 +60395,7 @@
         <v>7.6212009143717101E-4</v>
       </c>
     </row>
-    <row r="35" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.35">
       <c r="F35">
         <v>2.72</v>
       </c>
@@ -60409,7 +60415,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="36" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.35">
       <c r="F36">
         <v>6.7879236430252298E-3</v>
       </c>
@@ -60429,7 +60435,7 @@
         <v>0.10151727174955601</v>
       </c>
     </row>
-    <row r="37" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.35">
       <c r="F37">
         <v>1.86</v>
       </c>
@@ -60449,7 +60455,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="38" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.35">
       <c r="F38">
         <v>6.3022601977501799E-2</v>
       </c>
@@ -60469,82 +60475,239 @@
         <v>0.229212653279359</v>
       </c>
     </row>
-    <row r="40" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F40" t="str">
-        <f>IF(F34&lt;0.001,"***",IF(F34&lt;0.01,"**",IF(F34&lt;0.05,"*")))</f>
+    <row r="39" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="F40" s="17">
+        <f>ROUND(F33, 2)</f>
+        <v>2.74</v>
+      </c>
+      <c r="G40" s="17">
+        <f t="shared" ref="G40:K40" si="6">ROUND(G33, 2)</f>
+        <v>2.66</v>
+      </c>
+      <c r="H40" s="17">
+        <f t="shared" si="6"/>
+        <v>3.18</v>
+      </c>
+      <c r="I40" s="17">
+        <f t="shared" si="6"/>
+        <v>2.58</v>
+      </c>
+      <c r="J40" s="17">
+        <f t="shared" si="6"/>
+        <v>3.13</v>
+      </c>
+      <c r="K40" s="17">
+        <f t="shared" si="6"/>
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F41" s="12" t="str">
+        <f t="shared" ref="F41:K41" si="7">IF(F34&lt;0.001,"***",IF(F34&lt;0.01,"**",IF(F34&lt;0.05,"*")))</f>
         <v>**</v>
       </c>
-      <c r="G40" t="str">
-        <f t="shared" ref="G40:K40" si="6">IF(G34&lt;0.001,"***",IF(G34&lt;0.01,"**",IF(G34&lt;0.05,"*")))</f>
+      <c r="G41" s="7" t="str">
+        <f t="shared" si="7"/>
         <v>**</v>
       </c>
-      <c r="H40" t="str">
-        <f t="shared" si="6"/>
+      <c r="H41" s="7" t="str">
+        <f t="shared" si="7"/>
         <v>**</v>
       </c>
-      <c r="I40" t="str">
-        <f t="shared" si="6"/>
+      <c r="I41" s="7" t="str">
+        <f t="shared" si="7"/>
         <v>*</v>
       </c>
-      <c r="J40" t="str">
-        <f t="shared" si="6"/>
+      <c r="J41" s="7" t="str">
+        <f t="shared" si="7"/>
         <v>**</v>
       </c>
-      <c r="K40" t="str">
-        <f t="shared" si="6"/>
+      <c r="K41" s="13" t="str">
+        <f t="shared" si="7"/>
         <v>***</v>
       </c>
     </row>
-    <row r="41" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F41" t="b">
-        <f t="shared" ref="F41:K41" si="7">IF(F35&lt;0.001,"***",IF(F35&lt;0.01,"**",IF(F35&lt;0.05,"*")))</f>
-        <v>0</v>
-      </c>
-      <c r="G41" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H41" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I41" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J41" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K41" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F42" t="str">
-        <f t="shared" ref="F42:K42" si="8">IF(F36&lt;0.001,"***",IF(F36&lt;0.01,"**",IF(F36&lt;0.05,"*")))</f>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="F42" s="17">
+        <f>ROUND(F35, 2)</f>
+        <v>2.72</v>
+      </c>
+      <c r="G42" s="17">
+        <f t="shared" ref="G42:K42" si="8">ROUND(G35, 2)</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H42" s="17">
+        <f t="shared" si="8"/>
+        <v>3.89</v>
+      </c>
+      <c r="I42" s="17">
+        <f t="shared" si="8"/>
+        <v>2.27</v>
+      </c>
+      <c r="J42" s="17">
+        <f t="shared" si="8"/>
+        <v>2.19</v>
+      </c>
+      <c r="K42" s="17">
+        <f t="shared" si="8"/>
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F43" s="12" t="str">
+        <f>IF(F36&lt;0.001,"***",IF(F36&lt;0.01,"**",IF(F36&lt;0.05,"*")))</f>
         <v>**</v>
       </c>
-      <c r="G42" t="str">
-        <f t="shared" si="8"/>
+      <c r="G43" s="7" t="str">
+        <f>IF(G36&lt;0.001,"***",IF(G36&lt;0.01,"**",IF(G36&lt;0.05,"*")))</f>
         <v>*</v>
       </c>
-      <c r="H42" t="str">
-        <f t="shared" si="8"/>
+      <c r="H43" s="7" t="str">
+        <f>IF(H36&lt;0.001,"***",IF(H36&lt;0.01,"**",IF(H36&lt;0.05,"*")))</f>
         <v>***</v>
       </c>
-      <c r="I42" t="str">
-        <f t="shared" si="8"/>
+      <c r="I43" s="7" t="str">
+        <f>IF(I36&lt;0.001,"***",IF(I36&lt;0.01,"**",IF(I36&lt;0.05,"*")))</f>
         <v>*</v>
       </c>
-      <c r="J42" t="str">
-        <f t="shared" si="8"/>
+      <c r="J43" s="7" t="str">
+        <f>IF(J36&lt;0.001,"***",IF(J36&lt;0.01,"**",IF(J36&lt;0.05,"*")))</f>
         <v>*</v>
       </c>
-      <c r="K42" t="b">
-        <f t="shared" si="8"/>
-        <v>0</v>
+      <c r="K43" s="14">
+        <f>ROUND(K36, 2)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="F44" s="17">
+        <f>ROUND(F37, 2)</f>
+        <v>1.86</v>
+      </c>
+      <c r="G44" s="17">
+        <f t="shared" ref="G44:K44" si="9">ROUND(G37, 2)</f>
+        <v>1.71</v>
+      </c>
+      <c r="H44" s="17">
+        <f t="shared" si="9"/>
+        <v>3.22</v>
+      </c>
+      <c r="I44" s="17">
+        <f t="shared" si="9"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J44" s="17">
+        <f t="shared" si="9"/>
+        <v>2.41</v>
+      </c>
+      <c r="K44" s="17">
+        <f t="shared" si="9"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F45" s="14">
+        <f>ROUND(F38, 2)</f>
+        <v>0.06</v>
+      </c>
+      <c r="G45" s="14">
+        <f>ROUND(G38, 2)</f>
+        <v>0.09</v>
+      </c>
+      <c r="H45" s="15" t="str">
+        <f>IF(H38&lt;0.001,"***",IF(H38&lt;0.01,"**",IF(H38&lt;0.05,"*")))</f>
+        <v>**</v>
+      </c>
+      <c r="I45" s="14">
+        <f>ROUND(I38, 2)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J45" s="15" t="str">
+        <f>IF(J38&lt;0.001,"***",IF(J38&lt;0.01,"**",IF(J38&lt;0.05,"*")))</f>
+        <v>*</v>
+      </c>
+      <c r="K45" s="14">
+        <f>ROUND(K38, 2)</f>
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D48" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D51">
+        <v>9</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D53">
+        <v>11</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D55">
+        <v>13</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D56">
+        <v>14</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E57">
+        <f>SUM(E49:E56)</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Augmented DM and t-tests. Bfr correction on CY scaling from PNG.
</commit_message>
<xml_diff>
--- a/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
+++ b/models/NarxModelSearch/benchmarksIslandsVsRS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madks\Documents\GitHub\Ozone-Narx-DNN\models\NarxModelSearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C919F68-0D22-4363-B8DF-01EF1723F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4337454C-8E05-493E-B463-0E135736C37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18720" tabRatio="440" activeTab="4" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="440" activeTab="4" xr2:uid="{61FBCCFF-D26E-44A9-A7DF-005C2E7C4778}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosenbrock" sheetId="5" r:id="rId1"/>
@@ -59609,7 +59609,7 @@
   <dimension ref="D1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>